<commit_message>
Simulation A for AdjList complete
</commit_message>
<xml_diff>
--- a/Data/Scenarios/SIR Simulation/SIR Simulation.xlsx
+++ b/Data/Scenarios/SIR Simulation/SIR Simulation.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marto\git\Algos_Assignment1\Data\Scenarios\SIR Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A96AD1-AC1F-4AB6-B732-ACC4F4D194E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B8B91C-CC22-479D-AE59-BD2E234F2F3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12588" yWindow="300" windowWidth="21252" windowHeight="13608" activeTab="1" xr2:uid="{841EE581-550A-4663-911C-8BAD89104151}"/>
+    <workbookView xWindow="24540" yWindow="180" windowWidth="21252" windowHeight="13608" activeTab="1" xr2:uid="{841EE581-550A-4663-911C-8BAD89104151}"/>
   </bookViews>
   <sheets>
     <sheet name="File Structure" sheetId="2" r:id="rId1"/>
     <sheet name="AdjList - SimA" sheetId="1" r:id="rId2"/>
+    <sheet name="AdjMat - SimA" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="66">
   <si>
     <t xml:space="preserve">number of infected </t>
   </si>
@@ -230,6 +231,9 @@
   </si>
   <si>
     <t>Random</t>
+  </si>
+  <si>
+    <t>Total Infections Reached</t>
   </si>
 </sst>
 </file>
@@ -267,7 +271,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -275,21 +279,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,10 +853,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067A507A-BFD8-434A-A69D-E813FD95FEC4}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="X20" sqref="X20:X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,34 +870,45 @@
     <col min="13" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F2" s="3" t="s">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="P2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2"/>
       <c r="F3" t="s">
         <v>4</v>
       </c>
@@ -908,49 +936,103 @@
       <c r="N3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="P3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>25</v>
       </c>
@@ -963,8 +1045,62 @@
       <c r="D5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>1.8978598999999999E-2</v>
+      </c>
+      <c r="G5">
+        <v>2.2874228E-2</v>
+      </c>
+      <c r="H5">
+        <v>2.4041575999999999E-2</v>
+      </c>
+      <c r="I5">
+        <v>3.468297E-2</v>
+      </c>
+      <c r="J5">
+        <v>8.6951711000000001E-2</v>
+      </c>
+      <c r="K5">
+        <v>7.1584843999999995E-2</v>
+      </c>
+      <c r="L5">
+        <v>0.116804882</v>
+      </c>
+      <c r="M5">
+        <v>0.133218277</v>
+      </c>
+      <c r="N5">
+        <v>0.15941488000000001</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>346</v>
+      </c>
+      <c r="R5">
+        <v>403</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>4077</v>
+      </c>
+      <c r="V5">
+        <v>3317</v>
+      </c>
+      <c r="W5">
+        <v>6943</v>
+      </c>
+      <c r="X5">
+        <v>8181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>25</v>
       </c>
@@ -977,8 +1113,62 @@
       <c r="D6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>1.4876706999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>1.8157935E-2</v>
+      </c>
+      <c r="H6">
+        <v>2.2576539999999999E-2</v>
+      </c>
+      <c r="I6">
+        <v>3.9137765999999997E-2</v>
+      </c>
+      <c r="J6">
+        <v>5.4214024999999999E-2</v>
+      </c>
+      <c r="K6">
+        <v>8.3572379000000002E-2</v>
+      </c>
+      <c r="L6">
+        <v>6.0110342999999997E-2</v>
+      </c>
+      <c r="M6">
+        <v>0.10434732400000001</v>
+      </c>
+      <c r="N6">
+        <v>0.32169664599999998</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>368</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>3066</v>
+      </c>
+      <c r="U6">
+        <v>3828</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>6114</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>25</v>
       </c>
@@ -991,8 +1181,62 @@
       <c r="D7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>1.3901257E-2</v>
+      </c>
+      <c r="G7">
+        <v>1.8970462E-2</v>
+      </c>
+      <c r="H7">
+        <v>2.1973032999999999E-2</v>
+      </c>
+      <c r="I7">
+        <v>3.5547108000000001E-2</v>
+      </c>
+      <c r="J7">
+        <v>5.7180641999999997E-2</v>
+      </c>
+      <c r="K7">
+        <v>6.6199169000000002E-2</v>
+      </c>
+      <c r="L7">
+        <v>9.5662417999999999E-2</v>
+      </c>
+      <c r="M7">
+        <v>9.4558390000000006E-2</v>
+      </c>
+      <c r="N7">
+        <v>0.32116145400000001</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>269</v>
+      </c>
+      <c r="R7">
+        <v>359</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>2720</v>
+      </c>
+      <c r="U7">
+        <v>3579</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>5462</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>50</v>
       </c>
@@ -1005,8 +1249,62 @@
       <c r="D8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>1.4265348000000001E-2</v>
+      </c>
+      <c r="G8">
+        <v>2.0942191999999998E-2</v>
+      </c>
+      <c r="H8">
+        <v>2.3332803999999999E-2</v>
+      </c>
+      <c r="I8">
+        <v>3.4616987000000002E-2</v>
+      </c>
+      <c r="J8">
+        <v>5.7972966000000001E-2</v>
+      </c>
+      <c r="K8">
+        <v>5.9243153E-2</v>
+      </c>
+      <c r="L8">
+        <v>5.1538494999999997E-2</v>
+      </c>
+      <c r="M8">
+        <v>0.11582179099999999</v>
+      </c>
+      <c r="N8">
+        <v>0.14689661600000001</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>373</v>
+      </c>
+      <c r="R8">
+        <v>423</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>3751</v>
+      </c>
+      <c r="U8">
+        <v>4301</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>7569</v>
+      </c>
+      <c r="X8">
+        <v>8644</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>50</v>
       </c>
@@ -1019,8 +1317,62 @@
       <c r="D9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>2.4581479999999999E-2</v>
+      </c>
+      <c r="G9">
+        <v>1.9146562999999998E-2</v>
+      </c>
+      <c r="H9">
+        <v>2.2023656999999999E-2</v>
+      </c>
+      <c r="I9">
+        <v>3.9648638E-2</v>
+      </c>
+      <c r="J9">
+        <v>5.8393024000000002E-2</v>
+      </c>
+      <c r="K9">
+        <v>7.6324059999999999E-2</v>
+      </c>
+      <c r="L9">
+        <v>5.2029715999999997E-2</v>
+      </c>
+      <c r="M9">
+        <v>0.10329886000000001</v>
+      </c>
+      <c r="N9">
+        <v>0.132791784</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>410</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>4220</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>7208</v>
+      </c>
+      <c r="X9">
+        <v>8353</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>50</v>
       </c>
@@ -1033,8 +1385,62 @@
       <c r="D10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>1.7406076999999999E-2</v>
+      </c>
+      <c r="G10">
+        <v>1.7292569000000001E-2</v>
+      </c>
+      <c r="H10">
+        <v>1.8851006999999999E-2</v>
+      </c>
+      <c r="I10">
+        <v>5.6480717E-2</v>
+      </c>
+      <c r="J10">
+        <v>4.2987717000000002E-2</v>
+      </c>
+      <c r="K10">
+        <v>6.7445196999999998E-2</v>
+      </c>
+      <c r="L10">
+        <v>7.3627692999999994E-2</v>
+      </c>
+      <c r="M10">
+        <v>0.12825887599999999</v>
+      </c>
+      <c r="N10">
+        <v>0.15830902599999999</v>
+      </c>
+      <c r="P10">
+        <v>170</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>411</v>
+      </c>
+      <c r="S10">
+        <v>1651</v>
+      </c>
+      <c r="T10">
+        <v>3440</v>
+      </c>
+      <c r="U10">
+        <v>4086</v>
+      </c>
+      <c r="V10">
+        <v>3330</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>8180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>75</v>
       </c>
@@ -1047,8 +1453,62 @@
       <c r="D11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>1.4466994E-2</v>
+      </c>
+      <c r="G11">
+        <v>2.1977900000000002E-2</v>
+      </c>
+      <c r="H11">
+        <v>2.0969870000000002E-2</v>
+      </c>
+      <c r="I11">
+        <v>4.3760227999999998E-2</v>
+      </c>
+      <c r="J11">
+        <v>6.9419317999999994E-2</v>
+      </c>
+      <c r="K11">
+        <v>6.1361999E-2</v>
+      </c>
+      <c r="L11">
+        <v>6.0355806999999997E-2</v>
+      </c>
+      <c r="M11">
+        <v>0.101893542</v>
+      </c>
+      <c r="N11">
+        <v>0.14401012399999999</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>436</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>3864</v>
+      </c>
+      <c r="U11">
+        <v>4373</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>7813</v>
+      </c>
+      <c r="X11">
+        <v>8766</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>75</v>
       </c>
@@ -1061,8 +1521,62 @@
       <c r="D12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>1.8741484999999999E-2</v>
+      </c>
+      <c r="G12">
+        <v>2.1319416000000001E-2</v>
+      </c>
+      <c r="H12">
+        <v>1.9798891999999998E-2</v>
+      </c>
+      <c r="I12">
+        <v>3.4866439999999999E-2</v>
+      </c>
+      <c r="J12">
+        <v>4.8847915999999998E-2</v>
+      </c>
+      <c r="K12">
+        <v>7.3450203000000006E-2</v>
+      </c>
+      <c r="L12">
+        <v>5.0880077000000003E-2</v>
+      </c>
+      <c r="M12">
+        <v>9.68136E-2</v>
+      </c>
+      <c r="N12">
+        <v>0.14111729000000001</v>
+      </c>
+      <c r="P12">
+        <v>210</v>
+      </c>
+      <c r="Q12">
+        <v>376</v>
+      </c>
+      <c r="R12">
+        <v>428</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>3797</v>
+      </c>
+      <c r="U12">
+        <v>4344</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>7667</v>
+      </c>
+      <c r="X12">
+        <v>8719</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>75</v>
       </c>
@@ -1075,35 +1589,100 @@
       <c r="D13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="F13">
+        <v>1.3935804E-2</v>
+      </c>
+      <c r="G13">
+        <v>1.8102915000000001E-2</v>
+      </c>
+      <c r="H13">
+        <v>2.0507746E-2</v>
+      </c>
+      <c r="I13">
+        <v>3.3151053999999999E-2</v>
+      </c>
+      <c r="J13">
+        <v>4.5939307999999998E-2</v>
+      </c>
+      <c r="K13">
+        <v>5.6960163000000001E-2</v>
+      </c>
+      <c r="L13">
+        <v>5.0841473999999998E-2</v>
+      </c>
+      <c r="M13">
+        <v>8.4323644000000003E-2</v>
+      </c>
+      <c r="N13">
+        <v>0.120692013</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>367</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>3740</v>
+      </c>
+      <c r="U13">
+        <v>4314</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>7575</v>
+      </c>
+      <c r="X13">
+        <v>8635</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F17" s="3" t="s">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="F17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="P17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="3"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2"/>
       <c r="F18" t="s">
         <v>4</v>
       </c>
@@ -1131,50 +1710,104 @@
       <c r="N18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="P18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>4</v>
+      </c>
+      <c r="R18" t="s">
+        <v>4</v>
+      </c>
+      <c r="S18" t="s">
+        <v>6</v>
+      </c>
+      <c r="T18" t="s">
+        <v>6</v>
+      </c>
+      <c r="U18" t="s">
+        <v>6</v>
+      </c>
+      <c r="V18" t="s">
+        <v>9</v>
+      </c>
+      <c r="W18" t="s">
+        <v>9</v>
+      </c>
+      <c r="X18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1" t="s">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="M19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="N19" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>25</v>
       </c>
@@ -1187,8 +1820,62 @@
       <c r="D20" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>1.4732252E-2</v>
+      </c>
+      <c r="G20">
+        <v>2.7506701000000001E-2</v>
+      </c>
+      <c r="H20">
+        <v>2.4822273999999998E-2</v>
+      </c>
+      <c r="I20">
+        <v>3.6613092E-2</v>
+      </c>
+      <c r="J20">
+        <v>7.3526724000000002E-2</v>
+      </c>
+      <c r="K20">
+        <v>7.8569783000000004E-2</v>
+      </c>
+      <c r="L20">
+        <v>0.36742036300000003</v>
+      </c>
+      <c r="M20">
+        <v>0.16815074199999999</v>
+      </c>
+      <c r="N20">
+        <v>0.21156999100000001</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>493</v>
+      </c>
+      <c r="R20">
+        <v>499</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>4953</v>
+      </c>
+      <c r="U20">
+        <v>4997</v>
+      </c>
+      <c r="V20">
+        <v>2673</v>
+      </c>
+      <c r="W20">
+        <v>9880</v>
+      </c>
+      <c r="X20">
+        <v>9997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>25</v>
       </c>
@@ -1201,8 +1888,62 @@
       <c r="D21" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>1.4240064E-2</v>
+      </c>
+      <c r="G21">
+        <v>2.3883596999999999E-2</v>
+      </c>
+      <c r="H21">
+        <v>2.2836781E-2</v>
+      </c>
+      <c r="I21">
+        <v>4.1298675999999999E-2</v>
+      </c>
+      <c r="J21">
+        <v>7.4676364999999995E-2</v>
+      </c>
+      <c r="K21">
+        <v>9.6628056000000004E-2</v>
+      </c>
+      <c r="L21">
+        <v>5.450953E-2</v>
+      </c>
+      <c r="M21">
+        <v>0.129585175</v>
+      </c>
+      <c r="N21">
+        <v>0.18342640299999999</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>469</v>
+      </c>
+      <c r="R21">
+        <v>498</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>4766</v>
+      </c>
+      <c r="U21">
+        <v>4991</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>9980</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>25</v>
       </c>
@@ -1215,8 +1956,62 @@
       <c r="D22" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>1.9014720999999998E-2</v>
+      </c>
+      <c r="G22">
+        <v>2.4800583000000001E-2</v>
+      </c>
+      <c r="H22">
+        <v>2.2387562999999999E-2</v>
+      </c>
+      <c r="I22">
+        <v>3.9797702999999997E-2</v>
+      </c>
+      <c r="J22">
+        <v>8.3355003999999996E-2</v>
+      </c>
+      <c r="K22">
+        <v>8.2645662999999994E-2</v>
+      </c>
+      <c r="L22">
+        <v>5.7351500999999999E-2</v>
+      </c>
+      <c r="M22">
+        <v>0.17863815999999999</v>
+      </c>
+      <c r="N22">
+        <v>0.21654938900000001</v>
+      </c>
+      <c r="P22">
+        <v>14</v>
+      </c>
+      <c r="Q22">
+        <v>439</v>
+      </c>
+      <c r="R22">
+        <v>493</v>
+      </c>
+      <c r="S22">
+        <v>2</v>
+      </c>
+      <c r="T22">
+        <v>4497</v>
+      </c>
+      <c r="U22">
+        <v>4960</v>
+      </c>
+      <c r="V22">
+        <v>3</v>
+      </c>
+      <c r="W22">
+        <v>8891</v>
+      </c>
+      <c r="X22">
+        <v>9936</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>50</v>
       </c>
@@ -1229,8 +2024,62 @@
       <c r="D23" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>1.4715674999999999E-2</v>
+      </c>
+      <c r="G23">
+        <v>3.0511832999999999E-2</v>
+      </c>
+      <c r="H23">
+        <v>2.3565078E-2</v>
+      </c>
+      <c r="I23">
+        <v>9.0466942999999994E-2</v>
+      </c>
+      <c r="J23">
+        <v>6.2079428999999998E-2</v>
+      </c>
+      <c r="K23">
+        <v>9.0168371999999997E-2</v>
+      </c>
+      <c r="L23">
+        <v>0.160630045</v>
+      </c>
+      <c r="M23">
+        <v>0.128704019</v>
+      </c>
+      <c r="N23">
+        <v>0.169046102</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>497</v>
+      </c>
+      <c r="R23">
+        <v>499</v>
+      </c>
+      <c r="S23">
+        <v>3220</v>
+      </c>
+      <c r="T23">
+        <v>4994</v>
+      </c>
+      <c r="U23">
+        <v>4999</v>
+      </c>
+      <c r="V23">
+        <v>6351</v>
+      </c>
+      <c r="W23">
+        <v>9982</v>
+      </c>
+      <c r="X23">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>50</v>
       </c>
@@ -1243,8 +2092,62 @@
       <c r="D24" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <v>1.8779334000000002E-2</v>
+      </c>
+      <c r="G24">
+        <v>2.2721620000000001E-2</v>
+      </c>
+      <c r="H24">
+        <v>2.2030470999999999E-2</v>
+      </c>
+      <c r="I24">
+        <v>4.0896407000000003E-2</v>
+      </c>
+      <c r="J24">
+        <v>6.1917884999999999E-2</v>
+      </c>
+      <c r="K24">
+        <v>6.7622526000000002E-2</v>
+      </c>
+      <c r="L24">
+        <v>5.0271352999999998E-2</v>
+      </c>
+      <c r="M24">
+        <v>0.110834883</v>
+      </c>
+      <c r="N24">
+        <v>0.19574623499999999</v>
+      </c>
+      <c r="P24">
+        <v>2</v>
+      </c>
+      <c r="Q24">
+        <v>496</v>
+      </c>
+      <c r="R24">
+        <v>499</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>4975</v>
+      </c>
+      <c r="U24">
+        <v>4999</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>9951</v>
+      </c>
+      <c r="X24">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>50</v>
       </c>
@@ -1257,8 +2160,62 @@
       <c r="D25" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <v>1.4399181E-2</v>
+      </c>
+      <c r="G25">
+        <v>2.1660175E-2</v>
+      </c>
+      <c r="H25">
+        <v>2.1536787000000002E-2</v>
+      </c>
+      <c r="I25">
+        <v>0.123867623</v>
+      </c>
+      <c r="J25">
+        <v>5.8026714E-2</v>
+      </c>
+      <c r="K25">
+        <v>6.2723171999999994E-2</v>
+      </c>
+      <c r="L25">
+        <v>5.4940455999999999E-2</v>
+      </c>
+      <c r="M25">
+        <v>0.111103128</v>
+      </c>
+      <c r="N25">
+        <v>0.14989069699999999</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>494</v>
+      </c>
+      <c r="R25">
+        <v>499</v>
+      </c>
+      <c r="S25">
+        <v>1108</v>
+      </c>
+      <c r="T25">
+        <v>4955</v>
+      </c>
+      <c r="U25">
+        <v>4999</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>9873</v>
+      </c>
+      <c r="X25">
+        <v>9998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>75</v>
       </c>
@@ -1271,8 +2228,62 @@
       <c r="D26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <v>2.3896384E-2</v>
+      </c>
+      <c r="G26">
+        <v>2.1960927000000002E-2</v>
+      </c>
+      <c r="H26">
+        <v>2.3021624000000001E-2</v>
+      </c>
+      <c r="I26">
+        <v>7.4236050999999997E-2</v>
+      </c>
+      <c r="J26">
+        <v>6.0715973999999999E-2</v>
+      </c>
+      <c r="K26">
+        <v>7.4998758999999998E-2</v>
+      </c>
+      <c r="L26">
+        <v>7.0197469999999998E-2</v>
+      </c>
+      <c r="M26">
+        <v>0.112048367</v>
+      </c>
+      <c r="N26">
+        <v>0.18281529899999999</v>
+      </c>
+      <c r="P26">
+        <v>377</v>
+      </c>
+      <c r="Q26">
+        <v>498</v>
+      </c>
+      <c r="R26">
+        <v>499</v>
+      </c>
+      <c r="S26">
+        <v>3689</v>
+      </c>
+      <c r="T26">
+        <v>4995</v>
+      </c>
+      <c r="U26">
+        <v>4999</v>
+      </c>
+      <c r="V26">
+        <v>2</v>
+      </c>
+      <c r="W26">
+        <v>9993</v>
+      </c>
+      <c r="X26">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>75</v>
       </c>
@@ -1285,8 +2296,62 @@
       <c r="D27" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <v>1.4568193E-2</v>
+      </c>
+      <c r="G27">
+        <v>1.9848155999999999E-2</v>
+      </c>
+      <c r="H27">
+        <v>2.0526585E-2</v>
+      </c>
+      <c r="I27">
+        <v>7.1165802E-2</v>
+      </c>
+      <c r="J27">
+        <v>5.4084106999999999E-2</v>
+      </c>
+      <c r="K27">
+        <v>5.9428603000000003E-2</v>
+      </c>
+      <c r="L27">
+        <v>5.7531515999999998E-2</v>
+      </c>
+      <c r="M27">
+        <v>0.106988268</v>
+      </c>
+      <c r="N27">
+        <v>0.159436948</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>496</v>
+      </c>
+      <c r="R27">
+        <v>499</v>
+      </c>
+      <c r="S27">
+        <v>3367</v>
+      </c>
+      <c r="T27">
+        <v>4995</v>
+      </c>
+      <c r="U27">
+        <v>4999</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>9989</v>
+      </c>
+      <c r="X27">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>75</v>
       </c>
@@ -1299,11 +2364,67 @@
       <c r="D28" t="s">
         <v>64</v>
       </c>
+      <c r="F28">
+        <v>2.0846325999999998E-2</v>
+      </c>
+      <c r="G28">
+        <v>1.9991715E-2</v>
+      </c>
+      <c r="H28">
+        <v>2.0194705E-2</v>
+      </c>
+      <c r="I28">
+        <v>7.0565207000000005E-2</v>
+      </c>
+      <c r="J28">
+        <v>5.1965471999999999E-2</v>
+      </c>
+      <c r="K28">
+        <v>6.5918298E-2</v>
+      </c>
+      <c r="L28">
+        <v>0.11711508499999999</v>
+      </c>
+      <c r="M28">
+        <v>9.0494651999999995E-2</v>
+      </c>
+      <c r="N28">
+        <v>0.13127920300000001</v>
+      </c>
+      <c r="P28">
+        <v>324</v>
+      </c>
+      <c r="Q28">
+        <v>496</v>
+      </c>
+      <c r="R28">
+        <v>499</v>
+      </c>
+      <c r="S28">
+        <v>3144</v>
+      </c>
+      <c r="T28">
+        <v>4990</v>
+      </c>
+      <c r="U28">
+        <v>4999</v>
+      </c>
+      <c r="V28">
+        <v>6433</v>
+      </c>
+      <c r="W28">
+        <v>9984</v>
+      </c>
+      <c r="X28">
+        <v>9999</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C18:D18"/>
+    <mergeCell ref="P2:X2"/>
+    <mergeCell ref="P17:X17"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F2:N2"/>
     <mergeCell ref="A3:B3"/>
@@ -1315,4 +2436,618 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A74650-3F61-4268-A5F3-688C3B6DF3DF}">
+  <dimension ref="A1:X28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" customWidth="1"/>
+    <col min="13" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="P2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>75</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <v>75</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>75</v>
+      </c>
+      <c r="B11">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>75</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>75</v>
+      </c>
+      <c r="B13">
+        <v>75</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="P17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" t="s">
+        <v>6</v>
+      </c>
+      <c r="L18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>4</v>
+      </c>
+      <c r="R18" t="s">
+        <v>4</v>
+      </c>
+      <c r="S18" t="s">
+        <v>6</v>
+      </c>
+      <c r="T18" t="s">
+        <v>6</v>
+      </c>
+      <c r="U18" t="s">
+        <v>6</v>
+      </c>
+      <c r="V18" t="s">
+        <v>9</v>
+      </c>
+      <c r="W18" t="s">
+        <v>9</v>
+      </c>
+      <c r="X18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>50</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>75</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>50</v>
+      </c>
+      <c r="B23">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>50</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>50</v>
+      </c>
+      <c r="B25">
+        <v>75</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>75</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>75</v>
+      </c>
+      <c r="B27">
+        <v>50</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>75</v>
+      </c>
+      <c r="B28">
+        <v>75</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="F17:N17"/>
+    <mergeCell ref="P17:X17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="F2:N2"/>
+    <mergeCell ref="P2:X2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>